<commit_message>
fix bug: refresh array every time before sorting
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardxie/IdeaProjects/INFO6205_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90773ECB-E6A3-D245-A1C9-9C5EFC6A58AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61675D0-FEA0-0A47-8478-1D5CA774E38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{0DF6AD37-3E53-A044-B77C-A09573CF8599}"/>
+    <workbookView xWindow="440" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0DF6AD37-3E53-A044-B77C-A09573CF8599}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,265 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
-  <si>
-    <t>2021-11-29 00:41:06 INFO  Benchmark_Timer - Begin run: msd with 5 runs</t>
-  </si>
-  <si>
-    <t>msd sort with 5 iteration and 250000 elements, the mean is 499.2539336 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:09 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>msd wordnode sort with 5 iteration and 250000 elements, the mean is 317.07120580000003 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:12 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
-  </si>
-  <si>
-    <t>tim sort with 5 iteration and 250000 elements, the mean is 115.2244858 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:13 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:14 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>quick sort with 5 iteration and 250000 elements, the mean is 267.2368592 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:14 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
-  </si>
-  <si>
-    <t>husky sort with 5 iteration and 250000 elements, the mean is 0.012692400000000001 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:16 INFO  Benchmark_Timer - Begin run: lsd with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd sort with 5 iteration and 250000 elements, the mean is 1199.9414358 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:24 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd wordnode sort with 5 iteration and 250000 elements, the mean is 818.387663 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:30 INFO  Benchmark_Timer - Begin run: msd with 5 runs</t>
-  </si>
-  <si>
-    <t>msd sort with 5 iteration and 500000 elements, the mean is 943.6935799999999 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:37 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>msd wordnode sort with 5 iteration and 500000 elements, the mean is 784.081538 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:42 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
-  </si>
-  <si>
-    <t>tim sort with 5 iteration and 500000 elements, the mean is 497.2850468 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:46 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:47 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:48 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:49 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>quick sort with 5 iteration and 500000 elements, the mean is 652.6341052 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:49 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
-  </si>
-  <si>
-    <t>husky sort with 5 iteration and 500000 elements, the mean is 0.0160244 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:41:53 INFO  Benchmark_Timer - Begin run: lsd with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd sort with 5 iteration and 500000 elements, the mean is 3176.6357316000003 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:42:14 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd wordnode sort with 5 iteration and 500000 elements, the mean is 1877.8105351999998 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:42:29 INFO  Benchmark_Timer - Begin run: msd with 5 runs</t>
-  </si>
-  <si>
-    <t>msd sort with 5 iteration and 1000000 elements, the mean is 2208.5761146 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:42:44 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>msd wordnode sort with 5 iteration and 1000000 elements, the mean is 1775.9472010000002 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:42:56 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
-  </si>
-  <si>
-    <t>tim sort with 5 iteration and 1000000 elements, the mean is 1375.9417435999999 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:07 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:08 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:10 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:12 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:13 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>quick sort with 5 iteration and 1000000 elements, the mean is 1678.7181496 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:15 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
-  </si>
-  <si>
-    <t>husky sort with 5 iteration and 1000000 elements, the mean is 0.0135192 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:43:21 INFO  Benchmark_Timer - Begin run: lsd with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd sort with 5 iteration and 1000000 elements, the mean is 7367.7638357999995 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:44:10 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd wordnode sort with 5 iteration and 1000000 elements, the mean is 4298.5889588 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:44:43 INFO  Benchmark_Timer - Begin run: msd with 5 runs</t>
-  </si>
-  <si>
-    <t>msd sort with 5 iteration and 2000000 elements, the mean is 11764.074305999999 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:46:06 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>msd wordnode sort with 5 iteration and 2000000 elements, the mean is 5140.2970598 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:46:40 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
-  </si>
-  <si>
-    <t>tim sort with 5 iteration and 2000000 elements, the mean is 3355.0503550000003 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:04 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:08 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:12 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:15 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:19 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>quick sort with 5 iteration and 2000000 elements, the mean is 3647.9292988 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:23 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
-  </si>
-  <si>
-    <t>husky sort with 5 iteration and 2000000 elements, the mean is 0.014824799999999999 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:47:37 INFO  Benchmark_Timer - Begin run: lsd with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd sort with 5 iteration and 2000000 elements, the mean is 14549.9587986 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:49:14 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd wordnode sort with 5 iteration and 2000000 elements, the mean is 10062.9148728 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:50:30 INFO  Benchmark_Timer - Begin run: msd with 5 runs</t>
-  </si>
-  <si>
-    <t>msd sort with 5 iteration and 4000000 elements, the mean is 20572.6756068 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:52:58 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>msd wordnode sort with 5 iteration and 4000000 elements, the mean is 9480.4612392 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:54:01 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
-  </si>
-  <si>
-    <t>tim sort with 5 iteration and 4000000 elements, the mean is 8349.259137 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:55:01 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:55:09 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:55:17 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:55:26 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:55:34 INFO  Benchmark_Timer - Begin run: quick with 1 runs</t>
-  </si>
-  <si>
-    <t>quick sort with 5 iteration and 4000000 elements, the mean is 8313.253268 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:55:42 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
-  </si>
-  <si>
-    <t>husky sort with 5 iteration and 4000000 elements, the mean is 0.0132222 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:56:14 INFO  Benchmark_Timer - Begin run: lsd with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd sort with 5 iteration and 4000000 elements, the mean is 31176.660695 ms</t>
-  </si>
-  <si>
-    <t>2021-11-29 00:59:41 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
-  </si>
-  <si>
-    <t>lsd wordnode sort with 5 iteration and 4000000 elements, the mean is 20217.3878138 ms</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>husky</t>
   </si>
@@ -339,6 +81,216 @@
   </si>
   <si>
     <t>4M</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:27 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd wordnode sort with 5 iteration and 250000 elements, the mean is 636.1559341999999 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:32 INFO  Benchmark_Timer - Begin run: msd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd bytenode sort with 5 iteration and 250000 elements, the mean is 192.6294906 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:33 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
+  </si>
+  <si>
+    <t>tim sort with 5 iteration and 250000 elements, the mean is 284.36066040000003 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:35 INFO  Benchmark_Timer - Begin run: quick with 5 runs</t>
+  </si>
+  <si>
+    <t>quick sort with 5 iteration and 250000 elements, the mean is 249.10828320000002 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:37 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
+  </si>
+  <si>
+    <t>husky sort with 5 iteration and 250000 elements, the mean is 0.0124562 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:42 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd wordnode sort with 5 iteration and 250000 elements, the mean is 1282.9894689999999 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:51 INFO  Benchmark_Timer - Begin run: lsd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd bytenode sort with 5 iteration and 250000 elements, the mean is 607.1977876 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:37:57 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd wordnode sort with 5 iteration and 500000 elements, the mean is 1233.248752 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:05 INFO  Benchmark_Timer - Begin run: msd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd bytenode sort with 5 iteration and 500000 elements, the mean is 473.31928099999993 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:09 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
+  </si>
+  <si>
+    <t>tim sort with 5 iteration and 500000 elements, the mean is 696.4309114 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:14 INFO  Benchmark_Timer - Begin run: quick with 5 runs</t>
+  </si>
+  <si>
+    <t>quick sort with 5 iteration and 500000 elements, the mean is 624.9647882 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:18 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
+  </si>
+  <si>
+    <t>husky sort with 5 iteration and 500000 elements, the mean is 0.0173348 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:29 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd wordnode sort with 5 iteration and 500000 elements, the mean is 2102.1771 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:44 INFO  Benchmark_Timer - Begin run: lsd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd bytenode sort with 5 iteration and 500000 elements, the mean is 1358.5017758 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:38:55 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd wordnode sort with 5 iteration and 1000000 elements, the mean is 2999.624805 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:39:16 INFO  Benchmark_Timer - Begin run: msd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd bytenode sort with 5 iteration and 1000000 elements, the mean is 813.5141962 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:39:22 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
+  </si>
+  <si>
+    <t>tim sort with 5 iteration and 1000000 elements, the mean is 1696.8842052 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:39:34 INFO  Benchmark_Timer - Begin run: quick with 5 runs</t>
+  </si>
+  <si>
+    <t>quick sort with 5 iteration and 1000000 elements, the mean is 1494.2399192 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:39:45 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
+  </si>
+  <si>
+    <t>husky sort with 5 iteration and 1000000 elements, the mean is 0.0145148 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:40:09 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd wordnode sort with 5 iteration and 1000000 elements, the mean is 5008.7798334 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:40:45 INFO  Benchmark_Timer - Begin run: lsd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd bytenode sort with 5 iteration and 1000000 elements, the mean is 2656.2189924 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:41:08 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd wordnode sort with 5 iteration and 2000000 elements, the mean is 5973.4745138 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:41:53 INFO  Benchmark_Timer - Begin run: msd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd bytenode sort with 5 iteration and 2000000 elements, the mean is 4776.2226488 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:42:26 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
+  </si>
+  <si>
+    <t>tim sort with 5 iteration and 2000000 elements, the mean is 3983.3544498 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:42:55 INFO  Benchmark_Timer - Begin run: quick with 5 runs</t>
+  </si>
+  <si>
+    <t>quick sort with 5 iteration and 2000000 elements, the mean is 4056.942118 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:43:24 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
+  </si>
+  <si>
+    <t>husky sort with 5 iteration and 2000000 elements, the mean is 0.016508600000000002 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:44:13 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd wordnode sort with 5 iteration and 2000000 elements, the mean is 9874.4291686 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:45:21 INFO  Benchmark_Timer - Begin run: lsd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd bytenode sort with 5 iteration and 2000000 elements, the mean is 4855.2632924 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:46:06 INFO  Benchmark_Timer - Begin run: msd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd wordnode sort with 5 iteration and 4000000 elements, the mean is 12619.7327056 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:47:36 INFO  Benchmark_Timer - Begin run: msd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>msd bytenode sort with 5 iteration and 4000000 elements, the mean is 6142.306283 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:48:20 INFO  Benchmark_Timer - Begin run: tim with 5 runs</t>
+  </si>
+  <si>
+    <t>tim sort with 5 iteration and 4000000 elements, the mean is 9508.014529 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:49:26 INFO  Benchmark_Timer - Begin run: quick with 5 runs</t>
+  </si>
+  <si>
+    <t>quick sort with 5 iteration and 4000000 elements, the mean is 9176.2472196 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:50:31 INFO  Benchmark_Timer - Begin run: husky with 5 runs</t>
+  </si>
+  <si>
+    <t>husky sort with 5 iteration and 4000000 elements, the mean is 0.0150398 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:52:05 INFO  Benchmark_Timer - Begin run: lsd wordnode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd wordnode sort with 5 iteration and 4000000 elements, the mean is 20291.499308399998 ms</t>
+  </si>
+  <si>
+    <t>2021-11-30 02:54:29 INFO  Benchmark_Timer - Begin run: lsd bytenode with 5 runs</t>
+  </si>
+  <si>
+    <t>lsd bytenode sort with 5 iteration and 4000000 elements, the mean is 7595.6058764 ms</t>
   </si>
 </sst>
 </file>
@@ -563,22 +515,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>tim</c:v>
+                  <c:v>msd</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>tim</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -590,25 +542,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.26924E-2</c:v>
+                  <c:v>1.2456200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.2244858</c:v>
+                  <c:v>192.6294906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267.23685920000003</c:v>
+                  <c:v>249.10828319999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>317.07120579999997</c:v>
+                  <c:v>284.36066039999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>499.25393359999998</c:v>
+                  <c:v>607.19778759999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>818.38766299999997</c:v>
+                  <c:v>636.15593419999902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1199.9414357999999</c:v>
+                  <c:v>1282.9894689999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -907,22 +859,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>msd</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>quick</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>tim</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -934,25 +886,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.32222E-2</c:v>
+                  <c:v>1.5039800000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8313.2532680000004</c:v>
+                  <c:v>6142.3062829999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8349.2591369999991</c:v>
+                  <c:v>7595.6058763999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9480.4612391999999</c:v>
+                  <c:v>9176.2472195999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20217.3878138</c:v>
+                  <c:v>9508.014529</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20572.6756068</c:v>
+                  <c:v>12619.732705599999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31176.660694999999</c:v>
+                  <c:v>20291.4993083999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,22 +1181,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>tim</c:v>
+                  <c:v>msd</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>tim</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>msd</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1256,25 +1208,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.6024400000000001E-2</c:v>
+                  <c:v>1.7334800000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>497.28504679999998</c:v>
+                  <c:v>473.31928099999902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>652.63410520000002</c:v>
+                  <c:v>624.96478820000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>784.08153800000002</c:v>
+                  <c:v>696.43091140000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>943.69357999999897</c:v>
+                  <c:v>1233.248752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1877.81053519999</c:v>
+                  <c:v>1358.5017757999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3176.6357315999999</c:v>
+                  <c:v>2102.1770999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1551,22 +1503,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>tim</c:v>
+                  <c:v>msd</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>tim</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1578,25 +1530,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.35192E-2</c:v>
+                  <c:v>1.45148E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1375.9417435999901</c:v>
+                  <c:v>813.51419620000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1678.7181496000001</c:v>
+                  <c:v>1494.2399192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1775.9472009999999</c:v>
+                  <c:v>1696.8842052</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2208.5761146</c:v>
+                  <c:v>2656.2189923999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4298.5889588</c:v>
+                  <c:v>2999.6248049999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7367.7638357999904</c:v>
+                  <c:v>5008.7798333999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1879,16 +1831,16 @@
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>msd</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1900,25 +1852,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.48247999999999E-2</c:v>
+                  <c:v>1.6508599999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3355.0503549999999</c:v>
+                  <c:v>3983.3544498000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3647.9292988000002</c:v>
+                  <c:v>4056.9421179999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5140.2970598000002</c:v>
+                  <c:v>4776.2226487999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10062.9148728</c:v>
+                  <c:v>4855.2632924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11764.0743059999</c:v>
+                  <c:v>5973.4745137999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14549.958798600001</c:v>
+                  <c:v>9874.4291685999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2195,22 +2147,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>msd</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>quick</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>tim</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2222,25 +2174,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.32222E-2</c:v>
+                  <c:v>1.5039800000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8313.2532680000004</c:v>
+                  <c:v>6142.3062829999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8349.2591369999991</c:v>
+                  <c:v>7595.6058763999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9480.4612391999999</c:v>
+                  <c:v>9176.2472195999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20217.3878138</c:v>
+                  <c:v>9508.014529</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20572.6756068</c:v>
+                  <c:v>12619.732705599999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31176.660694999999</c:v>
+                  <c:v>20291.4993083999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2537,22 +2489,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>tim</c:v>
+                  <c:v>msd</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>tim</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2564,25 +2516,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.26924E-2</c:v>
+                  <c:v>1.2456200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.2244858</c:v>
+                  <c:v>192.6294906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267.23685920000003</c:v>
+                  <c:v>249.10828319999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>317.07120579999997</c:v>
+                  <c:v>284.36066039999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>499.25393359999998</c:v>
+                  <c:v>607.19778759999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>818.38766299999997</c:v>
+                  <c:v>636.15593419999902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1199.9414357999999</c:v>
+                  <c:v>1282.9894689999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2881,22 +2833,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>tim</c:v>
+                  <c:v>msd</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>tim</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>msd</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2908,25 +2860,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.6024400000000001E-2</c:v>
+                  <c:v>1.7334800000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>497.28504679999998</c:v>
+                  <c:v>473.31928099999902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>652.63410520000002</c:v>
+                  <c:v>624.96478820000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>784.08153800000002</c:v>
+                  <c:v>696.43091140000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>943.69357999999897</c:v>
+                  <c:v>1233.248752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1877.81053519999</c:v>
+                  <c:v>1358.5017757999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3176.6357315999999</c:v>
+                  <c:v>2102.1770999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3203,22 +3155,22 @@
                   <c:v>husky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>tim</c:v>
+                  <c:v>msd</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>tim</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3230,25 +3182,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.35192E-2</c:v>
+                  <c:v>1.45148E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1375.9417435999901</c:v>
+                  <c:v>813.51419620000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1678.7181496000001</c:v>
+                  <c:v>1494.2399192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1775.9472009999999</c:v>
+                  <c:v>1696.8842052</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2208.5761146</c:v>
+                  <c:v>2656.2189923999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4298.5889588</c:v>
+                  <c:v>2999.6248049999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7367.7638357999904</c:v>
+                  <c:v>5008.7798333999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3531,16 +3483,16 @@
                   <c:v>quick</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>msd</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>lsd</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>msd wordnode</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>lsd wordnode</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>msd</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lsd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3552,25 +3504,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.48247999999999E-2</c:v>
+                  <c:v>1.6508599999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3355.0503549999999</c:v>
+                  <c:v>3983.3544498000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3647.9292988000002</c:v>
+                  <c:v>4056.9421179999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5140.2970598000002</c:v>
+                  <c:v>4776.2226487999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10062.9148728</c:v>
+                  <c:v>4855.2632924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11764.0743059999</c:v>
+                  <c:v>5973.4745137999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14549.958798600001</c:v>
+                  <c:v>9874.4291685999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5438,10 +5390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CB103C-8443-424D-A2A2-87484E9B3E9C}">
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5451,698 +5403,622 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" t="s">
-        <v>86</v>
-      </c>
       <c r="K1">
-        <v>1.26924E-2</v>
+        <v>1.2456200000000001E-2</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="K2">
-        <v>115.2244858</v>
+        <v>192.6294906</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
-        <v>88</v>
-      </c>
       <c r="K3">
-        <v>267.23685920000003</v>
+        <v>249.10828319999999</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>317.07120579999997</v>
+        <v>284.36066039999997</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="K5">
-        <v>499.25393359999998</v>
+        <v>607.19778759999997</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>818.38766299999997</v>
+        <v>636.15593419999902</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>1199.9414357999999</v>
+        <v>1282.9894689999901</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I25" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>1.6024400000000001E-2</v>
+        <v>1.7334800000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="J26">
-        <v>497.28504679999998</v>
+        <v>473.31928099999902</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="I27" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="J27">
-        <v>652.63410520000002</v>
+        <v>624.96478820000004</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I28" t="s">
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="J28">
-        <v>784.08153800000002</v>
+        <v>696.43091140000001</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="I29" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="J29">
-        <v>943.69357999999897</v>
+        <v>1233.248752</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I30" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="J30">
-        <v>1877.81053519999</v>
+        <v>1358.5017757999999</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="J31">
-        <v>3176.6357315999999</v>
+        <v>2102.1770999999999</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="I50" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="I51" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="J51">
-        <v>1.35192E-2</v>
+        <v>1.45148E-2</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I52" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="J52">
-        <v>1375.9417435999901</v>
+        <v>813.51419620000001</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="I53" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="J53">
-        <v>1678.7181496000001</v>
+        <v>1494.2399192</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I54" t="s">
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="J54">
-        <v>1775.9472009999999</v>
+        <v>1696.8842052</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="I55" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="J55">
-        <v>2208.5761146</v>
+        <v>2656.2189923999999</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="I56" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="J56">
-        <v>4298.5889588</v>
+        <v>2999.6248049999999</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="I57" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="J57">
-        <v>7367.7638357999904</v>
+        <v>5008.7798333999999</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="I67" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="J68">
-        <v>1.48247999999999E-2</v>
+        <v>1.6508599999999998E-2</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
       <c r="J69">
-        <v>3355.0503549999999</v>
+        <v>3983.3544498000001</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="J70">
-        <v>3647.9292988000002</v>
+        <v>4056.9421179999999</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>66</v>
-      </c>
       <c r="I71" s="1" t="s">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="J71">
-        <v>5140.2970598000002</v>
+        <v>4776.2226487999997</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>67</v>
-      </c>
       <c r="I72" s="1" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="J72">
-        <v>10062.9148728</v>
+        <v>4855.2632924</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>68</v>
-      </c>
       <c r="I73" s="1" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="J73">
-        <v>11764.0743059999</v>
+        <v>5973.4745137999998</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>69</v>
-      </c>
       <c r="I74" s="1" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="J74">
-        <v>14549.958798600001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>76</v>
-      </c>
+        <v>9874.4291685999997</v>
+      </c>
+    </row>
+    <row r="81" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I81" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>77</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I82" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="J82">
-        <v>1.32222E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>78</v>
-      </c>
+        <v>1.5039800000000001E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I83" s="1" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="J83">
-        <v>8313.2532680000004</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>79</v>
-      </c>
+        <v>6142.3062829999999</v>
+      </c>
+    </row>
+    <row r="84" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I84" s="1" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="J84">
-        <v>8349.2591369999991</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>80</v>
-      </c>
+        <v>7595.6058763999999</v>
+      </c>
+    </row>
+    <row r="85" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I85" s="1" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="J85">
-        <v>9480.4612391999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>81</v>
-      </c>
+        <v>9176.2472195999999</v>
+      </c>
+    </row>
+    <row r="86" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I86" s="1" t="s">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="J86">
-        <v>20217.3878138</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>82</v>
-      </c>
+        <v>9508.014529</v>
+      </c>
+    </row>
+    <row r="87" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I87" s="1" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="J87">
-        <v>20572.6756068</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>83</v>
-      </c>
+        <v>12619.732705599999</v>
+      </c>
+    </row>
+    <row r="88" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I88" s="1" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="J88">
-        <v>31176.660694999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>85</v>
+        <v>20291.4993083999</v>
       </c>
     </row>
   </sheetData>
@@ -6158,8 +6034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7F059E-37E4-044E-887F-75528008D87B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
clean the code, upload sorted chinese character, complete unit test
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardxie/IdeaProjects/INFO6205_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289A919E-BCA2-4C47-806B-3A701D25079F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C578561-4BF3-6F4A-9905-70367DB723C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="1360" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{0DF6AD37-3E53-A044-B77C-A09573CF8599}"/>
+    <workbookView xWindow="6320" yWindow="1360" windowWidth="28040" windowHeight="17440" activeTab="8" xr2:uid="{0DF6AD37-3E53-A044-B77C-A09573CF8599}"/>
   </bookViews>
   <sheets>
     <sheet name="pinyin" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,9 @@
     <sheet name="pinyin chart" sheetId="4" r:id="rId4"/>
     <sheet name="husk chart" sheetId="6" r:id="rId5"/>
     <sheet name="byte chart" sheetId="2" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="byte vs pinyin" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v2.0" hidden="1">husk!$K$35:$K$37</definedName>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="170">
   <si>
     <t>husky</t>
   </si>
@@ -429,6 +431,132 @@
   </si>
   <si>
     <t>2021-12-02 23:52:06 INFO  Benchmark_Timer - Begin run: msd byte node and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>alex</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>parent name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>registration renewal?</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:02:37 INFO  Benchmark_Timer - Begin run: msd collator and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:02:52 INFO  Benchmark_Timer - Begin run: msd byte node and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:03:04 INFO  Benchmark_Timer - Begin run: tim and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:03:24 INFO  Benchmark_Timer - Begin run: quick and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:03:43 INFO  Benchmark_Timer - Begin run: husky and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:04:06 INFO  Benchmark_Timer - Begin run: lsd and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:04:32 INFO  Benchmark_Timer - Begin run: lsd byte node and 1000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:05:07 INFO  Benchmark_Timer - Begin run: msd collator and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:06:03 INFO  Benchmark_Timer - Begin run: msd byte node and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:06:40 INFO  Benchmark_Timer - Begin run: tim and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:07:10 INFO  Benchmark_Timer - Begin run: quick and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:07:38 INFO  Benchmark_Timer - Begin run: husky and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:08:10 INFO  Benchmark_Timer - Begin run: lsd and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:08:53 INFO  Benchmark_Timer - Begin run: lsd byte node and 1500000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:09:43 INFO  Benchmark_Timer - Begin run: msd collator and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:11:21 INFO  Benchmark_Timer - Begin run: msd byte node and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:12:25 INFO  Benchmark_Timer - Begin run: tim and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:13:08 INFO  Benchmark_Timer - Begin run: quick and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:13:45 INFO  Benchmark_Timer - Begin run: husky and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:14:26 INFO  Benchmark_Timer - Begin run: lsd and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:15:17 INFO  Benchmark_Timer - Begin run: lsd byte node and 2000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:16:18 INFO  Benchmark_Timer - Begin run: msd collator and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:18:18 INFO  Benchmark_Timer - Begin run: msd byte node and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:19:34 INFO  Benchmark_Timer - Begin run: tim and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:20:45 INFO  Benchmark_Timer - Begin run: quick and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:21:54 INFO  Benchmark_Timer - Begin run: husky and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:22:59 INFO  Benchmark_Timer - Begin run: lsd and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:24:18 INFO  Benchmark_Timer - Begin run: lsd byte node and 3000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:25:51 INFO  Benchmark_Timer - Begin run: msd collator and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:28:03 INFO  Benchmark_Timer - Begin run: msd byte node and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:29:24 INFO  Benchmark_Timer - Begin run: tim and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:30:53 INFO  Benchmark_Timer - Begin run: quick and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:32:25 INFO  Benchmark_Timer - Begin run: husky and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:34:00 INFO  Benchmark_Timer - Begin run: lsd and 4000000 elements with 10 runs</t>
+  </si>
+  <si>
+    <t>2021-12-03 18:35:51 INFO  Benchmark_Timer - Begin run: lsd byte node and 4000000 elements with 10 runs</t>
   </si>
 </sst>
 </file>
@@ -15064,8 +15192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DFAA4-4278-2343-9222-FFC4D5491D42}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15353,4 +15481,443 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68591A2-214D-2A4D-8652-40DD2CDE39B0}">
+  <dimension ref="C10:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCD8307-1D70-E04F-8265-F68C8EEABBC8}">
+  <dimension ref="A1:A75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1193.3312632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1002.4056785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1641.9662951999901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1622.5075199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1822.4092231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2211.5141911000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2211.5141911000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2907.9794781999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4668.5997549000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3066.8674141000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2464.0768904000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2373.0892391000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2705.8897711</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3514.3748728</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3514.3748728</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4113.3844971999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>8087.30639229999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5302.6826149999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3537.6140154999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3137.8088641999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3403.7592008000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4338.0417101000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4338.0417101000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5037.5307964000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>9824.8539834999992</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>6293.7061626000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5798.7852033999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5743.1479866</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>5414.9443593999904</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>6921.5136346999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>6921.5136346999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>7047.3616068000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>10782.457198100001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>6810.1976133999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>7405.5059007999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>7640.6832867000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>7924.4500300999898</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>9243.3009440999995</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>9243.3009440999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>8465.1165122000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>